<commit_message>
Updated project to fix some bugs
</commit_message>
<xml_diff>
--- a/Länderliste.xlsx
+++ b/Länderliste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18ef8cb8574601ad/Uni/Robotic Process Automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Documents\KYC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{F1B17AF5-9364-44AA-BB63-B3BE72DABE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FA5418E-2590-4806-AAD4-214C712775E9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812518D0-2E9A-4C13-9215-183418F2DABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{912CBF6D-28AD-482D-BD1E-0203146C039E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{912CBF6D-28AD-482D-BD1E-0203146C039E}"/>
   </bookViews>
   <sheets>
     <sheet name="countries" sheetId="2" r:id="rId1"/>
@@ -759,9 +759,6 @@
     <t>idn</t>
   </si>
   <si>
-    <t>Iran (Islamic Republic of)</t>
-  </si>
-  <si>
     <t>ir</t>
   </si>
   <si>
@@ -1807,6 +1804,9 @@
   </si>
   <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>Iran</t>
   </si>
 </sst>
 </file>
@@ -2202,8 +2202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8DB2C3-46FF-47F0-881D-00157F38977C}">
   <dimension ref="A1:E194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2228,7 +2228,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2245,7 +2245,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2262,7 +2262,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2279,7 +2279,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2296,7 +2296,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2313,7 +2313,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2330,7 +2330,7 @@
         <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2347,7 +2347,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2364,7 +2364,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2381,7 +2381,7 @@
         <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2398,7 +2398,7 @@
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2415,7 +2415,7 @@
         <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2432,7 +2432,7 @@
         <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2449,7 +2449,7 @@
         <v>42</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2466,7 +2466,7 @@
         <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2483,7 +2483,7 @@
         <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2500,7 +2500,7 @@
         <v>51</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>54</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2534,7 +2534,7 @@
         <v>57</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2551,7 +2551,7 @@
         <v>60</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2568,7 +2568,7 @@
         <v>63</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2585,7 +2585,7 @@
         <v>66</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2602,7 +2602,7 @@
         <v>69</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2619,7 +2619,7 @@
         <v>72</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2636,7 +2636,7 @@
         <v>75</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2653,7 +2653,7 @@
         <v>78</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2670,7 +2670,7 @@
         <v>81</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2687,7 +2687,7 @@
         <v>84</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2704,7 +2704,7 @@
         <v>87</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2721,7 +2721,7 @@
         <v>90</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2738,7 +2738,7 @@
         <v>93</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2755,7 +2755,7 @@
         <v>96</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2772,7 +2772,7 @@
         <v>99</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2789,7 +2789,7 @@
         <v>102</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2806,7 +2806,7 @@
         <v>105</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2823,7 +2823,7 @@
         <v>108</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2840,7 +2840,7 @@
         <v>111</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2857,7 +2857,7 @@
         <v>114</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2874,7 +2874,7 @@
         <v>117</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2891,7 +2891,7 @@
         <v>120</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2908,7 +2908,7 @@
         <v>123</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2925,7 +2925,7 @@
         <v>126</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2942,7 +2942,7 @@
         <v>129</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2959,7 +2959,7 @@
         <v>132</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2976,7 +2976,7 @@
         <v>135</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2993,7 +2993,7 @@
         <v>138</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3010,7 +3010,7 @@
         <v>141</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3027,7 +3027,7 @@
         <v>144</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3044,7 +3044,7 @@
         <v>147</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3061,7 +3061,7 @@
         <v>150</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3078,7 +3078,7 @@
         <v>153</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3095,7 +3095,7 @@
         <v>156</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3112,7 +3112,7 @@
         <v>159</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3129,7 +3129,7 @@
         <v>162</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3146,7 +3146,7 @@
         <v>165</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3163,7 +3163,7 @@
         <v>168</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3180,7 +3180,7 @@
         <v>171</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3197,7 +3197,7 @@
         <v>174</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3214,7 +3214,7 @@
         <v>177</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
         <v>180</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3248,7 +3248,7 @@
         <v>183</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3265,7 +3265,7 @@
         <v>186</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3282,7 +3282,7 @@
         <v>189</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3299,7 +3299,7 @@
         <v>192</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3316,7 +3316,7 @@
         <v>195</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3333,7 +3333,7 @@
         <v>198</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3350,7 +3350,7 @@
         <v>201</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3367,7 +3367,7 @@
         <v>204</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3384,7 +3384,7 @@
         <v>207</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3401,7 +3401,7 @@
         <v>210</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3418,7 +3418,7 @@
         <v>213</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3435,7 +3435,7 @@
         <v>216</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3452,7 +3452,7 @@
         <v>219</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3469,7 +3469,7 @@
         <v>222</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3486,7 +3486,7 @@
         <v>225</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3503,7 +3503,7 @@
         <v>228</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3520,7 +3520,7 @@
         <v>231</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3537,7 +3537,7 @@
         <v>234</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3554,7 +3554,7 @@
         <v>236</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3562,16 +3562,16 @@
         <v>364</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="E80" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3579,16 +3579,16 @@
         <v>368</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="E81" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3596,16 +3596,16 @@
         <v>372</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>245</v>
-      </c>
       <c r="E82" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3613,16 +3613,16 @@
         <v>376</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="E83" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3630,16 +3630,16 @@
         <v>380</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="E84" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3647,16 +3647,16 @@
         <v>388</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>254</v>
-      </c>
       <c r="E85" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3664,16 +3664,16 @@
         <v>392</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="E86" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3681,16 +3681,16 @@
         <v>400</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>260</v>
-      </c>
       <c r="E87" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3698,16 +3698,16 @@
         <v>398</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>263</v>
-      </c>
       <c r="E88" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3715,16 +3715,16 @@
         <v>404</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="E89" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3732,16 +3732,16 @@
         <v>296</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="E90" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3749,16 +3749,16 @@
         <v>408</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="E91" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3766,16 +3766,16 @@
         <v>410</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>275</v>
-      </c>
       <c r="E92" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3783,16 +3783,16 @@
         <v>414</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>278</v>
-      </c>
       <c r="E93" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3800,16 +3800,16 @@
         <v>417</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="D94" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>281</v>
-      </c>
       <c r="E94" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3817,16 +3817,16 @@
         <v>418</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="D95" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="E95" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3834,16 +3834,16 @@
         <v>428</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="D96" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>287</v>
-      </c>
       <c r="E96" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3851,16 +3851,16 @@
         <v>422</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>290</v>
-      </c>
       <c r="E97" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3868,16 +3868,16 @@
         <v>426</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D98" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="E98" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3885,16 +3885,16 @@
         <v>430</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>296</v>
-      </c>
       <c r="E99" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3902,16 +3902,16 @@
         <v>434</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="E100" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3919,16 +3919,16 @@
         <v>438</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>302</v>
-      </c>
       <c r="E101" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3936,16 +3936,16 @@
         <v>440</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>305</v>
-      </c>
       <c r="E102" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3953,16 +3953,16 @@
         <v>442</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="D103" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>308</v>
-      </c>
       <c r="E103" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3970,16 +3970,16 @@
         <v>450</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="D104" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="E104" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3987,16 +3987,16 @@
         <v>454</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="D105" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="D105" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="E105" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -4004,16 +4004,16 @@
         <v>458</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="D106" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D106" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="E106" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -4021,16 +4021,16 @@
         <v>462</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="D107" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D107" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="E107" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -4038,16 +4038,16 @@
         <v>466</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="D108" s="1" t="s">
-        <v>323</v>
-      </c>
       <c r="E108" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -4055,16 +4055,16 @@
         <v>470</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="D109" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>326</v>
-      </c>
       <c r="E109" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -4072,16 +4072,16 @@
         <v>584</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="D110" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>329</v>
-      </c>
       <c r="E110" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -4089,16 +4089,16 @@
         <v>478</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="D111" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="D111" s="1" t="s">
-        <v>332</v>
-      </c>
       <c r="E111" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -4106,16 +4106,16 @@
         <v>480</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="E112" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4123,16 +4123,16 @@
         <v>484</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="D113" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>338</v>
-      </c>
       <c r="E113" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4140,16 +4140,16 @@
         <v>583</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="D114" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>341</v>
-      </c>
       <c r="E114" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4157,16 +4157,16 @@
         <v>498</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>344</v>
-      </c>
       <c r="E115" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4174,16 +4174,16 @@
         <v>492</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="D116" s="1" t="s">
-        <v>347</v>
-      </c>
       <c r="E116" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4191,16 +4191,16 @@
         <v>496</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="D117" s="1" t="s">
-        <v>350</v>
-      </c>
       <c r="E117" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4208,16 +4208,16 @@
         <v>499</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>353</v>
-      </c>
       <c r="E118" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4225,16 +4225,16 @@
         <v>504</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="D119" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="D119" s="1" t="s">
-        <v>356</v>
-      </c>
       <c r="E119" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4242,16 +4242,16 @@
         <v>508</v>
       </c>
       <c r="B120" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="D120" s="1" t="s">
-        <v>359</v>
-      </c>
       <c r="E120" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4259,16 +4259,16 @@
         <v>104</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D121" s="1" t="s">
-        <v>362</v>
-      </c>
       <c r="E121" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4276,16 +4276,16 @@
         <v>516</v>
       </c>
       <c r="B122" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="D122" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="D122" s="1" t="s">
-        <v>365</v>
-      </c>
       <c r="E122" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4293,16 +4293,16 @@
         <v>520</v>
       </c>
       <c r="B123" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="D123" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="D123" s="1" t="s">
-        <v>368</v>
-      </c>
       <c r="E123" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -4310,16 +4310,16 @@
         <v>524</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>371</v>
-      </c>
       <c r="E124" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4327,16 +4327,16 @@
         <v>528</v>
       </c>
       <c r="B125" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="D125" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D125" s="1" t="s">
-        <v>374</v>
-      </c>
       <c r="E125" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4344,16 +4344,16 @@
         <v>554</v>
       </c>
       <c r="B126" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="D126" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="D126" s="1" t="s">
-        <v>377</v>
-      </c>
       <c r="E126" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4361,16 +4361,16 @@
         <v>558</v>
       </c>
       <c r="B127" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="D127" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="D127" s="1" t="s">
-        <v>380</v>
-      </c>
       <c r="E127" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4378,16 +4378,16 @@
         <v>562</v>
       </c>
       <c r="B128" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="D128" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>383</v>
-      </c>
       <c r="E128" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4395,16 +4395,16 @@
         <v>566</v>
       </c>
       <c r="B129" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="D129" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="D129" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="E129" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4412,16 +4412,16 @@
         <v>807</v>
       </c>
       <c r="B130" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="D130" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="D130" s="1" t="s">
-        <v>389</v>
-      </c>
       <c r="E130" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4429,16 +4429,16 @@
         <v>578</v>
       </c>
       <c r="B131" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="D131" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D131" s="1" t="s">
-        <v>392</v>
-      </c>
       <c r="E131" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4446,16 +4446,16 @@
         <v>512</v>
       </c>
       <c r="B132" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="D132" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="D132" s="1" t="s">
-        <v>395</v>
-      </c>
       <c r="E132" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4463,16 +4463,16 @@
         <v>586</v>
       </c>
       <c r="B133" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C133" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="D133" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="D133" s="1" t="s">
-        <v>398</v>
-      </c>
       <c r="E133" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4480,16 +4480,16 @@
         <v>585</v>
       </c>
       <c r="B134" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="D134" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="D134" s="1" t="s">
-        <v>401</v>
-      </c>
       <c r="E134" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4497,16 +4497,16 @@
         <v>591</v>
       </c>
       <c r="B135" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="D135" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="D135" s="1" t="s">
-        <v>404</v>
-      </c>
       <c r="E135" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4514,16 +4514,16 @@
         <v>598</v>
       </c>
       <c r="B136" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="D136" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D136" s="1" t="s">
-        <v>407</v>
-      </c>
       <c r="E136" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4531,16 +4531,16 @@
         <v>600</v>
       </c>
       <c r="B137" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C137" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="D137" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="D137" s="1" t="s">
-        <v>410</v>
-      </c>
       <c r="E137" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4548,16 +4548,16 @@
         <v>604</v>
       </c>
       <c r="B138" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="C138" s="1" t="s">
+      <c r="D138" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="D138" s="1" t="s">
-        <v>413</v>
-      </c>
       <c r="E138" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4565,16 +4565,16 @@
         <v>608</v>
       </c>
       <c r="B139" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C139" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="D139" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D139" s="1" t="s">
-        <v>416</v>
-      </c>
       <c r="E139" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4582,16 +4582,16 @@
         <v>616</v>
       </c>
       <c r="B140" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C140" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="D140" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="D140" s="1" t="s">
-        <v>419</v>
-      </c>
       <c r="E140" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4599,16 +4599,16 @@
         <v>620</v>
       </c>
       <c r="B141" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="D141" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>422</v>
-      </c>
       <c r="E141" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4616,16 +4616,16 @@
         <v>634</v>
       </c>
       <c r="B142" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C142" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="D142" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="D142" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="E142" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4633,16 +4633,16 @@
         <v>642</v>
       </c>
       <c r="B143" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C143" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="D143" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D143" s="1" t="s">
-        <v>428</v>
-      </c>
       <c r="E143" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4650,16 +4650,16 @@
         <v>643</v>
       </c>
       <c r="B144" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="D144" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="D144" s="1" t="s">
-        <v>431</v>
-      </c>
       <c r="E144" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4667,16 +4667,16 @@
         <v>646</v>
       </c>
       <c r="B145" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C145" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="D145" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="D145" s="1" t="s">
-        <v>434</v>
-      </c>
       <c r="E145" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4684,16 +4684,16 @@
         <v>659</v>
       </c>
       <c r="B146" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C146" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="D146" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="D146" s="1" t="s">
-        <v>437</v>
-      </c>
       <c r="E146" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4701,16 +4701,16 @@
         <v>662</v>
       </c>
       <c r="B147" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C147" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="D147" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="D147" s="1" t="s">
-        <v>440</v>
-      </c>
       <c r="E147" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4718,16 +4718,16 @@
         <v>670</v>
       </c>
       <c r="B148" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C148" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="D148" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="D148" s="1" t="s">
-        <v>443</v>
-      </c>
       <c r="E148" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4735,16 +4735,16 @@
         <v>882</v>
       </c>
       <c r="B149" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C149" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="D149" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="D149" s="1" t="s">
-        <v>446</v>
-      </c>
       <c r="E149" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4752,16 +4752,16 @@
         <v>674</v>
       </c>
       <c r="B150" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C150" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="D150" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="D150" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="E150" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4769,16 +4769,16 @@
         <v>678</v>
       </c>
       <c r="B151" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C151" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="D151" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="D151" s="1" t="s">
-        <v>452</v>
-      </c>
       <c r="E151" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4786,16 +4786,16 @@
         <v>682</v>
       </c>
       <c r="B152" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C152" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="D152" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="D152" s="1" t="s">
-        <v>455</v>
-      </c>
       <c r="E152" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4803,16 +4803,16 @@
         <v>686</v>
       </c>
       <c r="B153" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C153" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="D153" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="D153" s="1" t="s">
-        <v>458</v>
-      </c>
       <c r="E153" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4820,16 +4820,16 @@
         <v>688</v>
       </c>
       <c r="B154" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C154" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C154" s="1" t="s">
+      <c r="D154" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="D154" s="1" t="s">
-        <v>461</v>
-      </c>
       <c r="E154" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4837,16 +4837,16 @@
         <v>690</v>
       </c>
       <c r="B155" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C155" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="C155" s="1" t="s">
+      <c r="D155" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="D155" s="1" t="s">
-        <v>464</v>
-      </c>
       <c r="E155" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4854,16 +4854,16 @@
         <v>694</v>
       </c>
       <c r="B156" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C156" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="D156" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="D156" s="1" t="s">
-        <v>467</v>
-      </c>
       <c r="E156" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4871,16 +4871,16 @@
         <v>702</v>
       </c>
       <c r="B157" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C157" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C157" s="1" t="s">
+      <c r="D157" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="D157" s="1" t="s">
-        <v>470</v>
-      </c>
       <c r="E157" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4888,16 +4888,16 @@
         <v>703</v>
       </c>
       <c r="B158" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C158" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="D158" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="D158" s="1" t="s">
-        <v>473</v>
-      </c>
       <c r="E158" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4905,16 +4905,16 @@
         <v>705</v>
       </c>
       <c r="B159" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C159" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="D159" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="D159" s="1" t="s">
-        <v>476</v>
-      </c>
       <c r="E159" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4922,16 +4922,16 @@
         <v>90</v>
       </c>
       <c r="B160" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C160" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="C160" s="1" t="s">
+      <c r="D160" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="D160" s="1" t="s">
-        <v>479</v>
-      </c>
       <c r="E160" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4939,16 +4939,16 @@
         <v>706</v>
       </c>
       <c r="B161" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C161" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="D161" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="D161" s="1" t="s">
-        <v>482</v>
-      </c>
       <c r="E161" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4956,16 +4956,16 @@
         <v>710</v>
       </c>
       <c r="B162" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C162" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="C162" s="1" t="s">
+      <c r="D162" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="D162" s="1" t="s">
-        <v>485</v>
-      </c>
       <c r="E162" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4973,16 +4973,16 @@
         <v>728</v>
       </c>
       <c r="B163" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C163" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="C163" s="1" t="s">
+      <c r="D163" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="D163" s="1" t="s">
-        <v>488</v>
-      </c>
       <c r="E163" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4990,16 +4990,16 @@
         <v>724</v>
       </c>
       <c r="B164" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C164" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="C164" s="1" t="s">
+      <c r="D164" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="D164" s="1" t="s">
-        <v>491</v>
-      </c>
       <c r="E164" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -5007,16 +5007,16 @@
         <v>144</v>
       </c>
       <c r="B165" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C165" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="C165" s="1" t="s">
+      <c r="D165" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="D165" s="1" t="s">
-        <v>494</v>
-      </c>
       <c r="E165" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5024,16 +5024,16 @@
         <v>729</v>
       </c>
       <c r="B166" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C166" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="C166" s="1" t="s">
+      <c r="D166" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="D166" s="1" t="s">
-        <v>497</v>
-      </c>
       <c r="E166" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5041,16 +5041,16 @@
         <v>740</v>
       </c>
       <c r="B167" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C167" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="C167" s="1" t="s">
+      <c r="D167" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="D167" s="1" t="s">
-        <v>500</v>
-      </c>
       <c r="E167" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -5058,16 +5058,16 @@
         <v>752</v>
       </c>
       <c r="B168" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C168" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="C168" s="1" t="s">
+      <c r="D168" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="D168" s="1" t="s">
-        <v>503</v>
-      </c>
       <c r="E168" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -5075,16 +5075,16 @@
         <v>756</v>
       </c>
       <c r="B169" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C169" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="C169" s="1" t="s">
+      <c r="D169" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="D169" s="1" t="s">
-        <v>506</v>
-      </c>
       <c r="E169" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -5092,16 +5092,16 @@
         <v>760</v>
       </c>
       <c r="B170" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C170" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="D170" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="D170" s="1" t="s">
-        <v>509</v>
-      </c>
       <c r="E170" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -5109,16 +5109,16 @@
         <v>762</v>
       </c>
       <c r="B171" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C171" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="C171" s="1" t="s">
+      <c r="D171" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="D171" s="1" t="s">
-        <v>512</v>
-      </c>
       <c r="E171" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -5126,16 +5126,16 @@
         <v>834</v>
       </c>
       <c r="B172" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C172" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C172" s="1" t="s">
+      <c r="D172" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D172" s="1" t="s">
-        <v>515</v>
-      </c>
       <c r="E172" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -5143,16 +5143,16 @@
         <v>764</v>
       </c>
       <c r="B173" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C173" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="C173" s="1" t="s">
+      <c r="D173" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="D173" s="1" t="s">
-        <v>518</v>
-      </c>
       <c r="E173" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -5160,16 +5160,16 @@
         <v>626</v>
       </c>
       <c r="B174" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C174" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="C174" s="1" t="s">
+      <c r="D174" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D174" s="1" t="s">
-        <v>521</v>
-      </c>
       <c r="E174" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -5177,16 +5177,16 @@
         <v>768</v>
       </c>
       <c r="B175" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C175" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C175" s="1" t="s">
+      <c r="D175" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="D175" s="1" t="s">
-        <v>524</v>
-      </c>
       <c r="E175" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -5194,16 +5194,16 @@
         <v>776</v>
       </c>
       <c r="B176" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C176" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="C176" s="1" t="s">
+      <c r="D176" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="D176" s="1" t="s">
-        <v>527</v>
-      </c>
       <c r="E176" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5211,16 +5211,16 @@
         <v>780</v>
       </c>
       <c r="B177" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C177" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="C177" s="1" t="s">
+      <c r="D177" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="D177" s="1" t="s">
-        <v>530</v>
-      </c>
       <c r="E177" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5228,16 +5228,16 @@
         <v>788</v>
       </c>
       <c r="B178" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C178" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="C178" s="1" t="s">
+      <c r="D178" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="D178" s="1" t="s">
-        <v>533</v>
-      </c>
       <c r="E178" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -5245,16 +5245,16 @@
         <v>792</v>
       </c>
       <c r="B179" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C179" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="C179" s="1" t="s">
+      <c r="D179" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="D179" s="1" t="s">
-        <v>536</v>
-      </c>
       <c r="E179" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -5262,16 +5262,16 @@
         <v>795</v>
       </c>
       <c r="B180" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C180" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="C180" s="1" t="s">
+      <c r="D180" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="D180" s="1" t="s">
-        <v>539</v>
-      </c>
       <c r="E180" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -5279,16 +5279,16 @@
         <v>798</v>
       </c>
       <c r="B181" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C181" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="C181" s="1" t="s">
+      <c r="D181" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="D181" s="1" t="s">
-        <v>542</v>
-      </c>
       <c r="E181" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -5296,16 +5296,16 @@
         <v>800</v>
       </c>
       <c r="B182" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C182" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="C182" s="1" t="s">
+      <c r="D182" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="D182" s="1" t="s">
-        <v>545</v>
-      </c>
       <c r="E182" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5313,16 +5313,16 @@
         <v>804</v>
       </c>
       <c r="B183" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C183" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="C183" s="1" t="s">
+      <c r="D183" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="D183" s="1" t="s">
-        <v>548</v>
-      </c>
       <c r="E183" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -5330,16 +5330,16 @@
         <v>784</v>
       </c>
       <c r="B184" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C184" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="C184" s="1" t="s">
+      <c r="D184" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="D184" s="1" t="s">
-        <v>551</v>
-      </c>
       <c r="E184" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5347,16 +5347,16 @@
         <v>826</v>
       </c>
       <c r="B185" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="C185" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="C185" s="1" t="s">
+      <c r="D185" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="D185" s="1" t="s">
-        <v>554</v>
-      </c>
       <c r="E185" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -5364,16 +5364,16 @@
         <v>840</v>
       </c>
       <c r="B186" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C186" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="C186" s="1" t="s">
+      <c r="D186" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="D186" s="1" t="s">
-        <v>557</v>
-      </c>
       <c r="E186" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -5381,16 +5381,16 @@
         <v>858</v>
       </c>
       <c r="B187" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C187" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="C187" s="1" t="s">
+      <c r="D187" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="D187" s="1" t="s">
-        <v>560</v>
-      </c>
       <c r="E187" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -5398,16 +5398,16 @@
         <v>860</v>
       </c>
       <c r="B188" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="C188" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="C188" s="1" t="s">
+      <c r="D188" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="D188" s="1" t="s">
-        <v>563</v>
-      </c>
       <c r="E188" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5415,16 +5415,16 @@
         <v>548</v>
       </c>
       <c r="B189" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C189" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="C189" s="1" t="s">
+      <c r="D189" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="D189" s="1" t="s">
-        <v>566</v>
-      </c>
       <c r="E189" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5432,16 +5432,16 @@
         <v>862</v>
       </c>
       <c r="B190" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C190" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="C190" s="1" t="s">
+      <c r="D190" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="D190" s="1" t="s">
-        <v>569</v>
-      </c>
       <c r="E190" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5449,16 +5449,16 @@
         <v>704</v>
       </c>
       <c r="B191" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C191" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="C191" s="1" t="s">
+      <c r="D191" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="D191" s="1" t="s">
-        <v>572</v>
-      </c>
       <c r="E191" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5466,16 +5466,16 @@
         <v>887</v>
       </c>
       <c r="B192" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="C192" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="C192" s="1" t="s">
+      <c r="D192" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="D192" s="1" t="s">
-        <v>575</v>
-      </c>
       <c r="E192" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -5483,16 +5483,16 @@
         <v>894</v>
       </c>
       <c r="B193" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C193" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="C193" s="1" t="s">
+      <c r="D193" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="D193" s="1" t="s">
-        <v>578</v>
-      </c>
       <c r="E193" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5500,16 +5500,16 @@
         <v>716</v>
       </c>
       <c r="B194" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="C194" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="C194" s="1" t="s">
+      <c r="D194" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="D194" s="1" t="s">
-        <v>581</v>
-      </c>
       <c r="E194" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>